<commit_message>
Updates in Regitration and AccountSuccesPage with add on some WebElements and Methods
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestData.xlsx
+++ b/src/main/java/testData/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheerendra\eclipse-workspace\Pract\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9219209-71D7-4569-BCA6-BDAC2B29C695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC11B02-3F00-4FA9-96B1-FB5BF7E491DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3588" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -641,4 +642,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B077B49-ABC9-4E01-AAA0-3FD34BFFE106}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>